<commit_message>
Data analysis documents uploaded
</commit_message>
<xml_diff>
--- a/rubinius_rubinius_sequencing/OM-distances2.xlsx
+++ b/rubinius_rubinius_sequencing/OM-distances2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="0" windowWidth="24800" windowHeight="18580" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="0" windowWidth="24880" windowHeight="15560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="OM-distances2.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>V1</t>
   </si>
@@ -76,6 +76,60 @@
   </si>
   <si>
     <t>V19</t>
+  </si>
+  <si>
+    <t>2011-06</t>
+  </si>
+  <si>
+    <t>2011-07</t>
+  </si>
+  <si>
+    <t>2011-08</t>
+  </si>
+  <si>
+    <t>2011-09</t>
+  </si>
+  <si>
+    <t>2011-10</t>
+  </si>
+  <si>
+    <t>2011-11</t>
+  </si>
+  <si>
+    <t>2011-12</t>
+  </si>
+  <si>
+    <t>2012-01</t>
+  </si>
+  <si>
+    <t>2012-02</t>
+  </si>
+  <si>
+    <t>2012-03</t>
+  </si>
+  <si>
+    <t>2012-04</t>
+  </si>
+  <si>
+    <t>2012-05</t>
+  </si>
+  <si>
+    <t>2012-06</t>
+  </si>
+  <si>
+    <t>2012-07</t>
+  </si>
+  <si>
+    <t>2012-08</t>
+  </si>
+  <si>
+    <t>2012-09</t>
+  </si>
+  <si>
+    <t>2012-10</t>
+  </si>
+  <si>
+    <t>2012-11</t>
   </si>
 </sst>
 </file>
@@ -251,6 +305,10 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -260,6 +318,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Evolutionary rate</c:v>
+          </c:tx>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -268,6 +329,68 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="0"/>
           </c:trendline>
+          <c:cat>
+            <c:strRef>
+              <c:f>'OM-distances2.csv'!$E$30:$E$47</c:f>
+              <c:strCache>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>2011-06</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2011-07</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2011-08</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2011-09</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2011-10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2011-11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2011-12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2012-01</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2012-02</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2012-03</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2012-04</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2012-05</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2012-06</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2012-07</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2012-08</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2012-09</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2012-10</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2012-11</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'OM-distances2.csv'!$C$25:$T$25</c:f>
@@ -340,11 +463,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="596607848"/>
-        <c:axId val="580821400"/>
+        <c:axId val="690064152"/>
+        <c:axId val="668562248"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="596607848"/>
+        <c:axId val="690064152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -353,7 +476,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="580821400"/>
+        <c:crossAx val="668562248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -361,7 +484,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="580821400"/>
+        <c:axId val="668562248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -372,7 +495,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="596607848"/>
+        <c:crossAx val="690064152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -751,10 +874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T25"/>
+  <dimension ref="A1:T47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="C21" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30:E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2049,6 +2172,96 @@
         <v>0.46925376181060902</v>
       </c>
       <c r="T25" s="2"/>
+    </row>
+    <row r="30" spans="1:20">
+      <c r="E30" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20">
+      <c r="E31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20">
+      <c r="E32" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="5:5">
+      <c r="E33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="5:5">
+      <c r="E34" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="5:5">
+      <c r="E35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="5:5">
+      <c r="E36" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="5:5">
+      <c r="E37" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="5:5">
+      <c r="E38" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="5:5">
+      <c r="E39" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="5:5">
+      <c r="E40" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="5:5">
+      <c r="E41" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="5:5">
+      <c r="E42" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="43" spans="5:5">
+      <c r="E43" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44" spans="5:5">
+      <c r="E44" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="45" spans="5:5">
+      <c r="E45" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="46" spans="5:5">
+      <c r="E46" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="5:5">
+      <c r="E47" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>